<commit_message>
Started to parse data, fixing player names to ensure an accurate merge Requires multiple commits as the changed data must be reflected in the git to properly parse.
</commit_message>
<xml_diff>
--- a/Data/SalaryData2024.xlsx
+++ b/Data/SalaryData2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quint\OneDrive\Desktop\Python\PassRusherProfile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81857E69-DD1B-45AC-AC8E-47A7147D93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA7A1D3-125E-43AA-A079-A008C6418B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{145E95C2-4CEE-4C00-8587-05CEAAFF428B}"/>
+    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="6918" xr2:uid="{145E95C2-4CEE-4C00-8587-05CEAAFF428B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,15 +215,9 @@
     <t>Lions</t>
   </si>
   <si>
-    <t>Matt Judon</t>
-  </si>
-  <si>
     <t>Falcons</t>
   </si>
   <si>
-    <t>Dorance Armstrong Jr.</t>
-  </si>
-  <si>
     <t>Commanders</t>
   </si>
   <si>
@@ -290,9 +284,6 @@
     <t>Marcus Davenport</t>
   </si>
   <si>
-    <t>Ogbonnia Okoronkwo</t>
-  </si>
-  <si>
     <t>Tyree Wilson</t>
   </si>
   <si>
@@ -410,9 +401,6 @@
     <t>Felix Anudike-Uzomah</t>
   </si>
   <si>
-    <t>Gregory Rousseau</t>
-  </si>
-  <si>
     <t>Odafe Oweh</t>
   </si>
   <si>
@@ -545,9 +533,6 @@
     <t>Chauncey Golston</t>
   </si>
   <si>
-    <t>Patrick Jones II</t>
-  </si>
-  <si>
     <t>Justin Eboigbe</t>
   </si>
   <si>
@@ -560,9 +545,6 @@
     <t>Khalid Kareem</t>
   </si>
   <si>
-    <t>Carlos Basham Jr.</t>
-  </si>
-  <si>
     <t>Baron Browning</t>
   </si>
   <si>
@@ -927,6 +909,24 @@
   </si>
   <si>
     <t>Free Agency</t>
+  </si>
+  <si>
+    <t>Greg Rousseau</t>
+  </si>
+  <si>
+    <t>Dorance Armstrong</t>
+  </si>
+  <si>
+    <t>boogie Basham</t>
+  </si>
+  <si>
+    <t>Ogbo Okoronkwo</t>
+  </si>
+  <si>
+    <t>Matthew Judon</t>
+  </si>
+  <si>
+    <t>Pat Jones II</t>
   </si>
 </sst>
 </file>
@@ -1304,12 +1304,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056453F3-443A-43CE-9113-6295878462E1}">
   <dimension ref="A1:J240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="20.734375" customWidth="1"/>
     <col min="10" max="10" width="12.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1324,19 +1325,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="G1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1966,10 +1967,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B26" t="s">
         <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
       </c>
       <c r="C26">
         <v>33</v>
@@ -1992,10 +1993,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>292</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>28</v>
@@ -2018,10 +2019,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>29</v>
@@ -2044,7 +2045,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>42</v>
@@ -2070,10 +2071,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>32</v>
@@ -2096,7 +2097,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2122,7 +2123,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
@@ -2148,7 +2149,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
@@ -2174,7 +2175,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -2200,7 +2201,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -2226,7 +2227,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
         <v>58</v>
@@ -2252,7 +2253,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -2278,10 +2279,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38">
         <v>28</v>
@@ -2304,10 +2305,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39">
         <v>30</v>
@@ -2330,10 +2331,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>28</v>
@@ -2356,7 +2357,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -2382,7 +2383,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
@@ -2408,10 +2409,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43">
         <v>29</v>
@@ -2434,7 +2435,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
         <v>58</v>
@@ -2460,7 +2461,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>294</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -2486,7 +2487,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -2512,10 +2513,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C47">
         <v>28</v>
@@ -2538,10 +2539,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C48">
         <v>30</v>
@@ -2564,7 +2565,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
@@ -2590,10 +2591,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C50">
         <v>31</v>
@@ -2616,10 +2617,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C51">
         <v>28</v>
@@ -2642,10 +2643,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C52">
         <v>34</v>
@@ -2668,10 +2669,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <v>30</v>
@@ -2694,7 +2695,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
         <v>28</v>
@@ -2720,7 +2721,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -2746,10 +2747,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C56">
         <v>25</v>
@@ -2772,10 +2773,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C57">
         <v>26</v>
@@ -2798,7 +2799,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B58" t="s">
         <v>42</v>
@@ -2824,10 +2825,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C59">
         <v>28</v>
@@ -2850,7 +2851,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
         <v>40</v>
@@ -2876,10 +2877,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C61">
         <v>25</v>
@@ -2902,10 +2903,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C62">
         <v>28</v>
@@ -2928,7 +2929,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B63" t="s">
         <v>30</v>
@@ -2954,7 +2955,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B64" t="s">
         <v>30</v>
@@ -2980,10 +2981,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C65">
         <v>27</v>
@@ -3006,10 +3007,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C66">
         <v>31</v>
@@ -3032,10 +3033,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C67">
         <v>26</v>
@@ -3058,10 +3059,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C68">
         <v>31</v>
@@ -3084,7 +3085,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B69" t="s">
         <v>30</v>
@@ -3110,7 +3111,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
         <v>33</v>
@@ -3136,7 +3137,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
         <v>22</v>
@@ -3162,7 +3163,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
         <v>54</v>
@@ -3188,7 +3189,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B73" t="s">
         <v>37</v>
@@ -3214,10 +3215,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C74">
         <v>27</v>
@@ -3240,7 +3241,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
         <v>42</v>
@@ -3266,10 +3267,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C76">
         <v>28</v>
@@ -3292,10 +3293,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C77">
         <v>24</v>
@@ -3318,10 +3319,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B78" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C78">
         <v>23</v>
@@ -3344,7 +3345,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>124</v>
+        <v>291</v>
       </c>
       <c r="B79" t="s">
         <v>35</v>
@@ -3370,10 +3371,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B80" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C80">
         <v>27</v>
@@ -3396,10 +3397,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C81">
         <v>26</v>
@@ -3422,7 +3423,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
         <v>35</v>
@@ -3448,7 +3449,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B83" t="s">
         <v>54</v>
@@ -3474,7 +3475,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B84" t="s">
         <v>45</v>
@@ -3500,10 +3501,10 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C85">
         <v>26</v>
@@ -3526,7 +3527,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B86" t="s">
         <v>54</v>
@@ -3552,10 +3553,10 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C87">
         <v>23</v>
@@ -3578,7 +3579,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B88" t="s">
         <v>45</v>
@@ -3604,7 +3605,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
         <v>25</v>
@@ -3630,10 +3631,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C90">
         <v>25</v>
@@ -3656,10 +3657,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C91">
         <v>26</v>
@@ -3682,7 +3683,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B92" t="s">
         <v>58</v>
@@ -3708,7 +3709,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B93" t="s">
         <v>40</v>
@@ -3734,10 +3735,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B94" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C94">
         <v>29</v>
@@ -3760,7 +3761,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B95" t="s">
         <v>51</v>
@@ -3786,10 +3787,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C96">
         <v>24</v>
@@ -3812,7 +3813,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B97" t="s">
         <v>13</v>
@@ -3838,7 +3839,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B98" t="s">
         <v>37</v>
@@ -3864,7 +3865,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B99" t="s">
         <v>51</v>
@@ -3890,10 +3891,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B100" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C100">
         <v>26</v>
@@ -3916,10 +3917,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B101" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C101">
         <v>24</v>
@@ -3942,7 +3943,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
@@ -3968,7 +3969,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B103" t="s">
         <v>49</v>
@@ -3994,7 +3995,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B104" t="s">
         <v>49</v>
@@ -4020,10 +4021,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B105" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C105">
         <v>24</v>
@@ -4046,7 +4047,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B106" t="s">
         <v>42</v>
@@ -4072,10 +4073,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B107" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C107">
         <v>24</v>
@@ -4098,10 +4099,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B108" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C108">
         <v>27</v>
@@ -4124,10 +4125,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C109">
         <v>27</v>
@@ -4145,15 +4146,15 @@
         <v>1002172</v>
       </c>
       <c r="H109" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B110" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C110">
         <v>26</v>
@@ -4176,7 +4177,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B111" t="s">
         <v>19</v>
@@ -4202,10 +4203,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B112" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C112">
         <v>26</v>
@@ -4228,7 +4229,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B113" t="s">
         <v>25</v>
@@ -4254,7 +4255,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B114" t="s">
         <v>33</v>
@@ -4280,10 +4281,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B115" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C115">
         <v>28</v>
@@ -4306,10 +4307,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B116" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C116">
         <v>30</v>
@@ -4332,7 +4333,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B117" t="s">
         <v>45</v>
@@ -4358,7 +4359,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B118" t="s">
         <v>22</v>
@@ -4384,7 +4385,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B119" t="s">
         <v>30</v>
@@ -4410,7 +4411,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B120" t="s">
         <v>19</v>
@@ -4436,7 +4437,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
@@ -4462,7 +4463,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B122" t="s">
         <v>51</v>
@@ -4488,7 +4489,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>169</v>
+        <v>296</v>
       </c>
       <c r="B123" t="s">
         <v>40</v>
@@ -4514,7 +4515,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B124" t="s">
         <v>37</v>
@@ -4540,10 +4541,10 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B125" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C125">
         <v>33</v>
@@ -4566,10 +4567,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B126" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C126">
         <v>28</v>
@@ -4592,10 +4593,10 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B127" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C127">
         <v>27</v>
@@ -4618,10 +4619,10 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>174</v>
+        <v>293</v>
       </c>
       <c r="B128" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C128">
         <v>28</v>
@@ -4644,10 +4645,10 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B129" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C129">
         <v>26</v>
@@ -4670,7 +4671,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B130" t="s">
         <v>25</v>
@@ -4696,10 +4697,10 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B131" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C131">
         <v>24</v>
@@ -4722,10 +4723,10 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B132" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C132">
         <v>26</v>
@@ -4748,7 +4749,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B133" t="s">
         <v>19</v>
@@ -4774,7 +4775,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
@@ -4800,7 +4801,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B135" t="s">
         <v>51</v>
@@ -4826,10 +4827,10 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B136" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C136">
         <v>28</v>
@@ -4852,10 +4853,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B137" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C137">
         <v>29</v>
@@ -4878,7 +4879,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B138" t="s">
         <v>58</v>
@@ -4904,7 +4905,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B139" t="s">
         <v>58</v>
@@ -4930,7 +4931,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B140" t="s">
         <v>30</v>
@@ -4956,10 +4957,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B141" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C141">
         <v>28</v>
@@ -4982,7 +4983,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B142" t="s">
         <v>8</v>
@@ -5008,7 +5009,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B143" t="s">
         <v>8</v>
@@ -5029,12 +5030,12 @@
         <v>0</v>
       </c>
       <c r="H143" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B144" t="s">
         <v>51</v>
@@ -5060,10 +5061,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B145" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C145">
         <v>26</v>
@@ -5086,7 +5087,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B146" t="s">
         <v>22</v>
@@ -5112,10 +5113,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B147" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C147">
         <v>27</v>
@@ -5138,7 +5139,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B148" t="s">
         <v>51</v>
@@ -5164,10 +5165,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B149" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C149">
         <v>25</v>
@@ -5190,7 +5191,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B150" t="s">
         <v>30</v>
@@ -5216,7 +5217,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B151" t="s">
         <v>35</v>
@@ -5242,7 +5243,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B152" t="s">
         <v>33</v>
@@ -5268,7 +5269,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B153" t="s">
         <v>37</v>
@@ -5294,10 +5295,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B154" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C154">
         <v>26</v>
@@ -5315,12 +5316,12 @@
         <v>0</v>
       </c>
       <c r="H154" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B155" t="s">
         <v>45</v>
@@ -5346,7 +5347,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B156" t="s">
         <v>33</v>
@@ -5372,7 +5373,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B157" t="s">
         <v>25</v>
@@ -5393,15 +5394,15 @@
         <v>8500</v>
       </c>
       <c r="H157" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B158" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C158">
         <v>25</v>
@@ -5424,10 +5425,10 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B159" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C159">
         <v>25</v>
@@ -5450,7 +5451,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B160" t="s">
         <v>11</v>
@@ -5476,7 +5477,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B161" t="s">
         <v>42</v>
@@ -5497,12 +5498,12 @@
         <v>0</v>
       </c>
       <c r="H161" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B162" t="s">
         <v>42</v>
@@ -5523,12 +5524,12 @@
         <v>0</v>
       </c>
       <c r="H162" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B163" t="s">
         <v>37</v>
@@ -5549,12 +5550,12 @@
         <v>0</v>
       </c>
       <c r="H163" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B164" t="s">
         <v>16</v>
@@ -5575,12 +5576,12 @@
         <v>0</v>
       </c>
       <c r="H164" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B165" t="s">
         <v>30</v>
@@ -5601,12 +5602,12 @@
         <v>0</v>
       </c>
       <c r="H165" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B166" t="s">
         <v>51</v>
@@ -5627,15 +5628,15 @@
         <v>0</v>
       </c>
       <c r="H166" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B167" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C167">
         <v>26</v>
@@ -5653,12 +5654,12 @@
         <v>0</v>
       </c>
       <c r="H167" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B168" t="s">
         <v>28</v>
@@ -5679,12 +5680,12 @@
         <v>0</v>
       </c>
       <c r="H168" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B169" t="s">
         <v>22</v>
@@ -5705,12 +5706,12 @@
         <v>0</v>
       </c>
       <c r="H169" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B170" t="s">
         <v>19</v>
@@ -5731,15 +5732,15 @@
         <v>0</v>
       </c>
       <c r="H170" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B171" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C171">
         <v>27</v>
@@ -5757,12 +5758,12 @@
         <v>0</v>
       </c>
       <c r="H171" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
@@ -5783,12 +5784,12 @@
         <v>0</v>
       </c>
       <c r="H172" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
@@ -5809,15 +5810,15 @@
         <v>0</v>
       </c>
       <c r="H173" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B174" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C174">
         <v>26</v>
@@ -5835,15 +5836,15 @@
         <v>271648</v>
       </c>
       <c r="H174" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B175" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C175">
         <v>23</v>
@@ -5866,7 +5867,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
@@ -5892,7 +5893,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B177" t="s">
         <v>30</v>
@@ -5913,15 +5914,15 @@
         <v>0</v>
       </c>
       <c r="H177" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B178" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C178">
         <v>27</v>
@@ -5939,15 +5940,15 @@
         <v>0</v>
       </c>
       <c r="H178" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B179" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C179">
         <v>26</v>
@@ -5965,15 +5966,15 @@
         <v>0</v>
       </c>
       <c r="H179" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B180" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C180">
         <v>28</v>
@@ -5991,12 +5992,12 @@
         <v>0</v>
       </c>
       <c r="H180" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B181" t="s">
         <v>30</v>
@@ -6017,12 +6018,12 @@
         <v>0</v>
       </c>
       <c r="H181" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B182" t="s">
         <v>22</v>
@@ -6048,7 +6049,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B183" t="s">
         <v>28</v>
@@ -6074,7 +6075,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B184" t="s">
         <v>5</v>
@@ -6095,12 +6096,12 @@
         <v>0</v>
       </c>
       <c r="H184" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B185" t="s">
         <v>33</v>
@@ -6121,15 +6122,15 @@
         <v>0</v>
       </c>
       <c r="H185" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B186" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C186">
         <v>26</v>
@@ -6152,7 +6153,7 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B187" t="s">
         <v>49</v>
@@ -6173,12 +6174,12 @@
         <v>0</v>
       </c>
       <c r="H187" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B188" t="s">
         <v>5</v>
@@ -6199,12 +6200,12 @@
         <v>0</v>
       </c>
       <c r="H188" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B189" t="s">
         <v>22</v>
@@ -6225,12 +6226,12 @@
         <v>0</v>
       </c>
       <c r="H189" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B190" t="s">
         <v>54</v>
@@ -6251,15 +6252,15 @@
         <v>0</v>
       </c>
       <c r="H190" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B191" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C191">
         <v>26</v>
@@ -6277,15 +6278,15 @@
         <v>0</v>
       </c>
       <c r="H191" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B192" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C192">
         <v>27</v>
@@ -6303,12 +6304,12 @@
         <v>0</v>
       </c>
       <c r="H192" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B193" t="s">
         <v>45</v>
@@ -6329,12 +6330,12 @@
         <v>0</v>
       </c>
       <c r="H193" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B194" t="s">
         <v>49</v>
@@ -6355,15 +6356,15 @@
         <v>0</v>
       </c>
       <c r="H194" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B195" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C195">
         <v>24</v>
@@ -6381,15 +6382,15 @@
         <v>220000</v>
       </c>
       <c r="H195" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B196" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C196">
         <v>25</v>
@@ -6407,12 +6408,12 @@
         <v>245000</v>
       </c>
       <c r="H196" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B197" t="s">
         <v>5</v>
@@ -6433,12 +6434,12 @@
         <v>120000</v>
       </c>
       <c r="H197" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B198" t="s">
         <v>58</v>
@@ -6459,12 +6460,12 @@
         <v>15000</v>
       </c>
       <c r="H198" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B199" t="s">
         <v>30</v>
@@ -6485,12 +6486,12 @@
         <v>70000</v>
       </c>
       <c r="H199" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B200" t="s">
         <v>54</v>
@@ -6511,12 +6512,12 @@
         <v>0</v>
       </c>
       <c r="H200" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B201" t="s">
         <v>37</v>
@@ -6537,12 +6538,12 @@
         <v>0</v>
       </c>
       <c r="H201" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B202" t="s">
         <v>5</v>
@@ -6568,10 +6569,10 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B203" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C203">
         <v>24</v>
@@ -6589,15 +6590,15 @@
         <v>0</v>
       </c>
       <c r="H203" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B204" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C204">
         <v>25</v>
@@ -6615,12 +6616,12 @@
         <v>0</v>
       </c>
       <c r="H204" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B205" t="s">
         <v>30</v>
@@ -6641,12 +6642,12 @@
         <v>0</v>
       </c>
       <c r="H205" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B206" t="s">
         <v>11</v>
@@ -6667,12 +6668,12 @@
         <v>0</v>
       </c>
       <c r="H206" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B207" t="s">
         <v>19</v>
@@ -6693,12 +6694,12 @@
         <v>0</v>
       </c>
       <c r="H207" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B208" t="s">
         <v>16</v>
@@ -6719,12 +6720,12 @@
         <v>0</v>
       </c>
       <c r="H208" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B209" t="s">
         <v>13</v>
@@ -6745,15 +6746,15 @@
         <v>0</v>
       </c>
       <c r="H209" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B210" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C210">
         <v>26</v>
@@ -6776,7 +6777,7 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B211" t="s">
         <v>28</v>
@@ -6797,15 +6798,15 @@
         <v>9000</v>
       </c>
       <c r="H211" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B212" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C212">
         <v>25</v>
@@ -6823,15 +6824,15 @@
         <v>2000</v>
       </c>
       <c r="H212" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B213" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C213">
         <v>26</v>
@@ -6849,12 +6850,12 @@
         <v>1000</v>
       </c>
       <c r="H213" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B214" t="s">
         <v>13</v>
@@ -6880,10 +6881,10 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B215" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C215">
         <v>24</v>
@@ -6901,15 +6902,15 @@
         <v>0</v>
       </c>
       <c r="H215" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B216" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C216">
         <v>26</v>
@@ -6927,12 +6928,12 @@
         <v>0</v>
       </c>
       <c r="H216" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B217" t="s">
         <v>40</v>
@@ -6953,15 +6954,15 @@
         <v>0</v>
       </c>
       <c r="H217" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B218" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C218">
         <v>26</v>
@@ -6979,15 +6980,15 @@
         <v>0</v>
       </c>
       <c r="H218" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B219" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C219">
         <v>27</v>
@@ -7005,12 +7006,12 @@
         <v>0</v>
       </c>
       <c r="H219" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B220" t="s">
         <v>28</v>
@@ -7031,15 +7032,15 @@
         <v>0</v>
       </c>
       <c r="H220" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B221" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C221">
         <v>25</v>
@@ -7057,12 +7058,12 @@
         <v>0</v>
       </c>
       <c r="H221" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B222" t="s">
         <v>37</v>
@@ -7083,12 +7084,12 @@
         <v>0</v>
       </c>
       <c r="H222" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B223" t="s">
         <v>16</v>
@@ -7109,12 +7110,12 @@
         <v>0</v>
       </c>
       <c r="H223" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B224" t="s">
         <v>16</v>
@@ -7135,15 +7136,15 @@
         <v>0</v>
       </c>
       <c r="H224" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B225" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C225">
         <v>26</v>
@@ -7161,15 +7162,15 @@
         <v>0</v>
       </c>
       <c r="H225" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B226" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C226">
         <v>24</v>
@@ -7187,12 +7188,12 @@
         <v>0</v>
       </c>
       <c r="H226" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B227" t="s">
         <v>40</v>
@@ -7213,12 +7214,12 @@
         <v>0</v>
       </c>
       <c r="H227" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B228" t="s">
         <v>22</v>
@@ -7239,12 +7240,12 @@
         <v>0</v>
       </c>
       <c r="H228" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B229" t="s">
         <v>19</v>
@@ -7265,12 +7266,12 @@
         <v>0</v>
       </c>
       <c r="H229" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B230" t="s">
         <v>5</v>
@@ -7291,12 +7292,12 @@
         <v>0</v>
       </c>
       <c r="H230" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B231" t="s">
         <v>25</v>
@@ -7317,12 +7318,12 @@
         <v>0</v>
       </c>
       <c r="H231" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B232" t="s">
         <v>5</v>
@@ -7343,12 +7344,12 @@
         <v>0</v>
       </c>
       <c r="H232" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B233" t="s">
         <v>58</v>
@@ -7369,15 +7370,15 @@
         <v>0</v>
       </c>
       <c r="H233" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B234" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C234">
         <v>25</v>
@@ -7395,15 +7396,15 @@
         <v>0</v>
       </c>
       <c r="H234" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B235" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C235">
         <v>25</v>
@@ -7421,15 +7422,15 @@
         <v>0</v>
       </c>
       <c r="H235" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B236" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C236">
         <v>28</v>
@@ -7447,12 +7448,12 @@
         <v>0</v>
       </c>
       <c r="H236" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B237" t="s">
         <v>28</v>
@@ -7473,15 +7474,15 @@
         <v>0</v>
       </c>
       <c r="H237" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B238" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C238">
         <v>25</v>
@@ -7499,12 +7500,12 @@
         <v>0</v>
       </c>
       <c r="H238" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B239" t="s">
         <v>58</v>
@@ -7525,12 +7526,12 @@
         <v>0</v>
       </c>
       <c r="H239" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B240" t="s">
         <v>45</v>
@@ -7551,10 +7552,11 @@
         <v>0</v>
       </c>
       <c r="H240" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Relevant salary data manually added to the appropriate excel file. It appears that recently retired players and players who recently restructured or signed new deals were not included in the original salary data and had to be added based on their 24-25 salary data
</commit_message>
<xml_diff>
--- a/Data/SalaryData2024.xlsx
+++ b/Data/SalaryData2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quint\OneDrive\Desktop\Python\PassRusherProfile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA7A1D3-125E-43AA-A079-A008C6418B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCF4517-737D-4132-A43C-A393B2195DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="6918" xr2:uid="{145E95C2-4CEE-4C00-8587-05CEAAFF428B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{145E95C2-4CEE-4C00-8587-05CEAAFF428B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="351">
   <si>
     <t>Player</t>
   </si>
@@ -927,6 +927,168 @@
   </si>
   <si>
     <t>Pat Jones II</t>
+  </si>
+  <si>
+    <t>Joey Bosa</t>
+  </si>
+  <si>
+    <t>Isaiah Land</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys</t>
+  </si>
+  <si>
+    <t>Jamie Sheriff</t>
+  </si>
+  <si>
+    <t>Miami Dolphins</t>
+  </si>
+  <si>
+    <t>Rashad Weaver</t>
+  </si>
+  <si>
+    <t>Tennessee Titans</t>
+  </si>
+  <si>
+    <t>Deatrich Wise Jr.</t>
+  </si>
+  <si>
+    <t>New England Patriots</t>
+  </si>
+  <si>
+    <t>Adetokunbo Ogundeji</t>
+  </si>
+  <si>
+    <t>Atlanta Falcons</t>
+  </si>
+  <si>
+    <t>Preston Smith</t>
+  </si>
+  <si>
+    <t>Green Bay Packers</t>
+  </si>
+  <si>
+    <t>Dre'Mont Jones</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks</t>
+  </si>
+  <si>
+    <t>Haason Reddick</t>
+  </si>
+  <si>
+    <t>Philadelphia Eagles</t>
+  </si>
+  <si>
+    <t>Sam Hubbard</t>
+  </si>
+  <si>
+    <t>Cincinnati Bengals</t>
+  </si>
+  <si>
+    <t>Chicago Bears</t>
+  </si>
+  <si>
+    <t>Zaven Collins</t>
+  </si>
+  <si>
+    <t>Arizona Cardinals</t>
+  </si>
+  <si>
+    <t>Nick Herbig</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers</t>
+  </si>
+  <si>
+    <t>DJ Coleman</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars</t>
+  </si>
+  <si>
+    <t>Charles Harris</t>
+  </si>
+  <si>
+    <t>Detroit Lions</t>
+  </si>
+  <si>
+    <t>Yannick Ngakoue</t>
+  </si>
+  <si>
+    <t>Michael Burton</t>
+  </si>
+  <si>
+    <t>Kansas City Chiefs</t>
+  </si>
+  <si>
+    <t>DeMarvin Leal</t>
+  </si>
+  <si>
+    <t>Jamin Davis</t>
+  </si>
+  <si>
+    <t>Washington Commanders</t>
+  </si>
+  <si>
+    <t>Adam Gotsis</t>
+  </si>
+  <si>
+    <t>Takk McKinley</t>
+  </si>
+  <si>
+    <t>Cam Gill</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>DeMarcus Walker</t>
+  </si>
+  <si>
+    <t>Marquis Haynes Sr.</t>
+  </si>
+  <si>
+    <t>Carolina Panthers</t>
+  </si>
+  <si>
+    <t>Efe Obada</t>
+  </si>
+  <si>
+    <t>Trevor Nowaske</t>
+  </si>
+  <si>
+    <t>Reggie Gilliam</t>
+  </si>
+  <si>
+    <t>Buffalo Bills</t>
+  </si>
+  <si>
+    <t>Harold Landry III</t>
+  </si>
+  <si>
+    <t>Los Angeles Chargers</t>
+  </si>
+  <si>
+    <t>Brent Urban</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens</t>
+  </si>
+  <si>
+    <t>Jermaine Johnson</t>
+  </si>
+  <si>
+    <t>New York Jets</t>
+  </si>
+  <si>
+    <t>Casey Toohill</t>
+  </si>
+  <si>
+    <t>Shaq Lawson</t>
+  </si>
+  <si>
+    <t>Joe Gaziano</t>
   </si>
 </sst>
 </file>
@@ -965,9 +1127,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1302,15 +1470,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056453F3-443A-43CE-9113-6295878462E1}">
-  <dimension ref="A1:J240"/>
+  <dimension ref="A1:J272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="J271" sqref="J271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20.734375" customWidth="1"/>
+    <col min="4" max="4" width="12.3125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7555,6 +7724,838 @@
         <v>252</v>
       </c>
     </row>
+    <row r="241" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A241" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C241" s="2">
+        <v>24</v>
+      </c>
+      <c r="D241" s="3">
+        <v>2705000</v>
+      </c>
+      <c r="E241" s="3">
+        <v>902000</v>
+      </c>
+      <c r="F241" s="3">
+        <v>45000</v>
+      </c>
+      <c r="G241" s="3">
+        <v>45000</v>
+      </c>
+      <c r="H241" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A242" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C242" s="2">
+        <v>23</v>
+      </c>
+      <c r="D242" s="3">
+        <v>2710000</v>
+      </c>
+      <c r="E242" s="3">
+        <v>903333</v>
+      </c>
+      <c r="F242" s="3">
+        <v>50000</v>
+      </c>
+      <c r="G242" s="3">
+        <v>50000</v>
+      </c>
+      <c r="H242" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A243" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C243" s="2">
+        <v>26</v>
+      </c>
+      <c r="D243" s="3">
+        <v>4100000</v>
+      </c>
+      <c r="E243" s="3">
+        <v>1025000</v>
+      </c>
+      <c r="F243" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G243" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H243" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A244" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C244" s="2">
+        <v>30</v>
+      </c>
+      <c r="D244" s="3">
+        <v>22000000</v>
+      </c>
+      <c r="E244" s="3">
+        <v>5500000</v>
+      </c>
+      <c r="F244" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="G244" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A245" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C245" s="2">
+        <v>26</v>
+      </c>
+      <c r="D245" s="3">
+        <v>3800000</v>
+      </c>
+      <c r="E245" s="3">
+        <v>950000</v>
+      </c>
+      <c r="F245" s="3">
+        <v>320000</v>
+      </c>
+      <c r="G245" s="3">
+        <v>320000</v>
+      </c>
+      <c r="H245" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A246" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C246" s="2">
+        <v>32</v>
+      </c>
+      <c r="D246" s="3">
+        <v>52000000</v>
+      </c>
+      <c r="E246" s="3">
+        <v>13000000</v>
+      </c>
+      <c r="F246" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="G246" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="H246" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A247" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C247" s="2">
+        <v>28</v>
+      </c>
+      <c r="D247" s="3">
+        <v>51530000</v>
+      </c>
+      <c r="E247" s="3">
+        <v>17176667</v>
+      </c>
+      <c r="F247" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="G247" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="H247" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A248" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C248" s="2">
+        <v>30</v>
+      </c>
+      <c r="D248" s="3">
+        <v>45000000</v>
+      </c>
+      <c r="E248" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="F248" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="G248" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="H248" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C249" s="2">
+        <v>29</v>
+      </c>
+      <c r="D249" s="3">
+        <v>40000000</v>
+      </c>
+      <c r="E249" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F249" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="G249" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="H249" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C250" s="2">
+        <v>25</v>
+      </c>
+      <c r="D250" s="3">
+        <v>14700000</v>
+      </c>
+      <c r="E250" s="3">
+        <v>3675000</v>
+      </c>
+      <c r="F250" s="3">
+        <v>14700000</v>
+      </c>
+      <c r="G250" s="3">
+        <v>14700000</v>
+      </c>
+      <c r="H250" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A251" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C251" s="2">
+        <v>24</v>
+      </c>
+      <c r="D251" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="E251" s="3">
+        <v>1250000</v>
+      </c>
+      <c r="F251" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G251" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H251" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C252" s="2">
+        <v>25</v>
+      </c>
+      <c r="D252" s="3">
+        <v>2570000</v>
+      </c>
+      <c r="E252" s="3">
+        <v>857000</v>
+      </c>
+      <c r="F252" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G252" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H252" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A253" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C253" s="2">
+        <v>30</v>
+      </c>
+      <c r="D253" s="3">
+        <v>13000000</v>
+      </c>
+      <c r="E253" s="3">
+        <v>6500000</v>
+      </c>
+      <c r="F253" s="3">
+        <v>7000000</v>
+      </c>
+      <c r="G253" s="3">
+        <v>7000000</v>
+      </c>
+      <c r="H253" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C254" s="2">
+        <v>30</v>
+      </c>
+      <c r="D254" s="3">
+        <v>10500000</v>
+      </c>
+      <c r="E254" s="3">
+        <v>10500000</v>
+      </c>
+      <c r="F254" s="3">
+        <v>10500000</v>
+      </c>
+      <c r="G254" s="3">
+        <v>10500000</v>
+      </c>
+      <c r="H254" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A255" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C255" s="2">
+        <v>34</v>
+      </c>
+      <c r="D255" s="3">
+        <v>2500000</v>
+      </c>
+      <c r="E255" s="3">
+        <v>1250000</v>
+      </c>
+      <c r="F255" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G255" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H255" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A256" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C256" s="2">
+        <v>24</v>
+      </c>
+      <c r="D256" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="E256" s="3">
+        <v>1250000</v>
+      </c>
+      <c r="F256" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G256" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H256" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A257" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C257" s="2">
+        <v>27</v>
+      </c>
+      <c r="D257" s="3">
+        <v>13800000</v>
+      </c>
+      <c r="E257" s="3">
+        <v>3450000</v>
+      </c>
+      <c r="F257" s="3">
+        <v>13800000</v>
+      </c>
+      <c r="G257" s="3">
+        <v>13800000</v>
+      </c>
+      <c r="H257" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A258" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C258" s="2">
+        <v>33</v>
+      </c>
+      <c r="D258" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="E258" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F258" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G258" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H258" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A259" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C259" s="2">
+        <v>29</v>
+      </c>
+      <c r="D259" s="3">
+        <v>4250000</v>
+      </c>
+      <c r="E259" s="3">
+        <v>4250000</v>
+      </c>
+      <c r="F259" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G259" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H259" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A260" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C260" s="2">
+        <v>27</v>
+      </c>
+      <c r="D260" s="3">
+        <v>2705000</v>
+      </c>
+      <c r="E260" s="3">
+        <v>902000</v>
+      </c>
+      <c r="F260" s="3">
+        <v>45000</v>
+      </c>
+      <c r="G260" s="3">
+        <v>45000</v>
+      </c>
+      <c r="H260" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A261" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C261" s="2">
+        <v>31</v>
+      </c>
+      <c r="D261" s="3">
+        <v>21000000</v>
+      </c>
+      <c r="E261" s="3">
+        <v>7000000</v>
+      </c>
+      <c r="F261" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="G261" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="H261" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A262" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C262" s="2">
+        <v>31</v>
+      </c>
+      <c r="D262" s="3">
+        <v>5500000</v>
+      </c>
+      <c r="E262" s="3">
+        <v>2750000</v>
+      </c>
+      <c r="F262" s="3">
+        <v>2300000</v>
+      </c>
+      <c r="G262" s="3">
+        <v>2300000</v>
+      </c>
+      <c r="H262" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A263" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C263" s="2">
+        <v>33</v>
+      </c>
+      <c r="D263" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="E263" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F263" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G263" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H263" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A264" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C264" s="2">
+        <v>24</v>
+      </c>
+      <c r="D264" s="3">
+        <v>2710000</v>
+      </c>
+      <c r="E264" s="3">
+        <v>903333</v>
+      </c>
+      <c r="F264" s="3">
+        <v>50000</v>
+      </c>
+      <c r="G264" s="3">
+        <v>50000</v>
+      </c>
+      <c r="H264" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A265" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C265" s="2">
+        <v>28</v>
+      </c>
+      <c r="D265" s="3">
+        <v>5200000</v>
+      </c>
+      <c r="E265" s="3">
+        <v>2600000</v>
+      </c>
+      <c r="F265" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G265" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H265" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A266" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C266" s="2">
+        <v>29</v>
+      </c>
+      <c r="D266" s="3">
+        <v>43500000</v>
+      </c>
+      <c r="E266" s="3">
+        <v>14500000</v>
+      </c>
+      <c r="F266" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="G266" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="H266" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A267" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C267" s="2">
+        <v>29</v>
+      </c>
+      <c r="D267" s="3">
+        <v>135000000</v>
+      </c>
+      <c r="E267" s="3">
+        <v>27000000</v>
+      </c>
+      <c r="F267" s="3">
+        <v>102000000</v>
+      </c>
+      <c r="G267" s="3">
+        <v>78000000</v>
+      </c>
+      <c r="H267" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A268" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C268" s="2">
+        <v>33</v>
+      </c>
+      <c r="D268" s="3">
+        <v>2500000</v>
+      </c>
+      <c r="E268" s="3">
+        <v>2500000</v>
+      </c>
+      <c r="F268" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G268" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H268" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A269" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C269" s="2">
+        <v>26</v>
+      </c>
+      <c r="D269" s="3">
+        <v>13088000</v>
+      </c>
+      <c r="E269" s="3">
+        <v>3272000</v>
+      </c>
+      <c r="F269" s="3">
+        <v>13088000</v>
+      </c>
+      <c r="G269" s="3">
+        <v>13088000</v>
+      </c>
+      <c r="H269" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A270" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C270" s="2">
+        <v>28</v>
+      </c>
+      <c r="D270" s="3">
+        <v>2700000</v>
+      </c>
+      <c r="E270" s="3">
+        <v>900000</v>
+      </c>
+      <c r="F270" s="3">
+        <v>150000</v>
+      </c>
+      <c r="G270" s="3">
+        <v>150000</v>
+      </c>
+      <c r="H270" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A271" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C271" s="2">
+        <v>31</v>
+      </c>
+      <c r="D271" s="3">
+        <v>9000000</v>
+      </c>
+      <c r="E271" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="F271" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="G271" s="3">
+        <v>3000000</v>
+      </c>
+      <c r="H271" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A272" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C272" s="2">
+        <v>27</v>
+      </c>
+      <c r="D272" s="3">
+        <v>2500000</v>
+      </c>
+      <c r="E272" s="3">
+        <v>833333</v>
+      </c>
+      <c r="F272" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G272" s="3">
+        <v>100000</v>
+      </c>
+      <c r="H272" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual addition of contract info, removed players without active snaps in 2024-2025 NFL season Reordered code structure for logical flow Created temporary code to ensure data sets matched with names. Explored utilizing 2023-2024 data for players without active snapcounts, but lack of data integrity made this impossible. Kept 2023 NFLdata for later iterations to add more longevity based stats, should it become valuable to the model.
</commit_message>
<xml_diff>
--- a/Data/SalaryData2024.xlsx
+++ b/Data/SalaryData2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quint\OneDrive\Desktop\Python\PassRusherProfile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCF4517-737D-4132-A43C-A393B2195DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301FCFF7-F4E0-4725-B059-9A3709163EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{145E95C2-4CEE-4C00-8587-05CEAAFF428B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="352">
   <si>
     <t>Player</t>
   </si>
@@ -984,6 +984,9 @@
   </si>
   <si>
     <t>Cincinnati Bengals</t>
+  </si>
+  <si>
+    <t>Khari Blasingame</t>
   </si>
   <si>
     <t>Chicago Bears</t>
@@ -1470,16 +1473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056453F3-443A-43CE-9113-6295878462E1}">
-  <dimension ref="A1:J272"/>
+  <dimension ref="A1:J273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="J271" sqref="J271"/>
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="J252" sqref="J252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20.734375" customWidth="1"/>
-    <col min="4" max="4" width="12.3125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7724,131 +7726,131 @@
         <v>252</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>299</v>
+        <v>344</v>
       </c>
       <c r="C241" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D241" s="3">
-        <v>2705000</v>
+        <v>135000000</v>
       </c>
       <c r="E241" s="3">
-        <v>902000</v>
+        <v>27000000</v>
       </c>
       <c r="F241" s="3">
-        <v>45000</v>
+        <v>102000000</v>
       </c>
       <c r="G241" s="3">
-        <v>45000</v>
+        <v>78000000</v>
       </c>
       <c r="H241" s="2" t="s">
-        <v>184</v>
+        <v>17</v>
       </c>
     </row>
     <row r="242" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="2" t="s">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>301</v>
+        <v>346</v>
       </c>
       <c r="C242" s="2">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D242" s="3">
-        <v>2710000</v>
+        <v>2500000</v>
       </c>
       <c r="E242" s="3">
-        <v>903333</v>
+        <v>2500000</v>
       </c>
       <c r="F242" s="3">
-        <v>50000</v>
+        <v>1000000</v>
       </c>
       <c r="G242" s="3">
-        <v>50000</v>
+        <v>1000000</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>184</v>
+        <v>52</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="2" t="s">
-        <v>302</v>
+        <v>347</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>303</v>
+        <v>348</v>
       </c>
       <c r="C243" s="2">
         <v>26</v>
       </c>
       <c r="D243" s="3">
-        <v>4100000</v>
+        <v>13088000</v>
       </c>
       <c r="E243" s="3">
-        <v>1025000</v>
+        <v>3272000</v>
       </c>
       <c r="F243" s="3">
-        <v>1000000</v>
+        <v>13088000</v>
       </c>
       <c r="G243" s="3">
-        <v>1000000</v>
+        <v>13088000</v>
       </c>
       <c r="H243" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A244" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C244" s="2">
+        <v>28</v>
+      </c>
+      <c r="D244" s="3">
+        <v>2700000</v>
+      </c>
+      <c r="E244" s="3">
+        <v>900000</v>
+      </c>
+      <c r="F244" s="3">
+        <v>150000</v>
+      </c>
+      <c r="G244" s="3">
+        <v>150000</v>
+      </c>
+      <c r="H244" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A244" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C244" s="2">
-        <v>30</v>
-      </c>
-      <c r="D244" s="3">
-        <v>22000000</v>
-      </c>
-      <c r="E244" s="3">
-        <v>5500000</v>
-      </c>
-      <c r="F244" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="G244" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="H244" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="2" t="s">
-        <v>306</v>
+        <v>350</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>307</v>
+        <v>342</v>
       </c>
       <c r="C245" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D245" s="3">
-        <v>3800000</v>
+        <v>9000000</v>
       </c>
       <c r="E245" s="3">
-        <v>950000</v>
+        <v>3000000</v>
       </c>
       <c r="F245" s="3">
-        <v>320000</v>
+        <v>3000000</v>
       </c>
       <c r="G245" s="3">
-        <v>320000</v>
+        <v>3000000</v>
       </c>
       <c r="H245" s="2" t="s">
         <v>52</v>
@@ -7856,207 +7858,207 @@
     </row>
     <row r="246" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="2" t="s">
-        <v>308</v>
+        <v>351</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C246" s="2">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D246" s="3">
-        <v>52000000</v>
+        <v>2500000</v>
       </c>
       <c r="E246" s="3">
-        <v>13000000</v>
+        <v>833333</v>
       </c>
       <c r="F246" s="3">
-        <v>16000000</v>
+        <v>100000</v>
       </c>
       <c r="G246" s="3">
-        <v>16000000</v>
+        <v>100000</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="2" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="C247" s="2">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D247" s="3">
-        <v>51530000</v>
+        <v>2705000</v>
       </c>
       <c r="E247" s="3">
-        <v>17176667</v>
+        <v>902000</v>
       </c>
       <c r="F247" s="3">
-        <v>30000000</v>
+        <v>45000</v>
       </c>
       <c r="G247" s="3">
-        <v>30000000</v>
+        <v>45000</v>
       </c>
       <c r="H247" s="2" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
     </row>
     <row r="248" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="2" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="C248" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D248" s="3">
-        <v>45000000</v>
+        <v>2710000</v>
       </c>
       <c r="E248" s="3">
-        <v>15000000</v>
+        <v>903333</v>
       </c>
       <c r="F248" s="3">
-        <v>30000000</v>
+        <v>50000</v>
       </c>
       <c r="G248" s="3">
-        <v>30000000</v>
+        <v>50000</v>
       </c>
       <c r="H248" s="2" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="2" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="C249" s="2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D249" s="3">
-        <v>40000000</v>
+        <v>4100000</v>
       </c>
       <c r="E249" s="3">
+        <v>1025000</v>
+      </c>
+      <c r="F249" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G249" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="H249" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C250" s="2">
+        <v>30</v>
+      </c>
+      <c r="D250" s="3">
+        <v>22000000</v>
+      </c>
+      <c r="E250" s="3">
+        <v>5500000</v>
+      </c>
+      <c r="F250" s="3">
         <v>10000000</v>
       </c>
-      <c r="F249" s="3">
-        <v>16000000</v>
-      </c>
-      <c r="G249" s="3">
-        <v>16000000</v>
-      </c>
-      <c r="H249" s="2" t="s">
+      <c r="G250" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="H250" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A250" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C250" s="2">
-        <v>25</v>
-      </c>
-      <c r="D250" s="3">
-        <v>14700000</v>
-      </c>
-      <c r="E250" s="3">
-        <v>3675000</v>
-      </c>
-      <c r="F250" s="3">
-        <v>14700000</v>
-      </c>
-      <c r="G250" s="3">
-        <v>14700000</v>
-      </c>
-      <c r="H250" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="251" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="2" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="C251" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D251" s="3">
-        <v>5000000</v>
+        <v>3800000</v>
       </c>
       <c r="E251" s="3">
-        <v>1250000</v>
+        <v>950000</v>
       </c>
       <c r="F251" s="3">
-        <v>3000000</v>
+        <v>320000</v>
       </c>
       <c r="G251" s="3">
-        <v>3000000</v>
+        <v>320000</v>
       </c>
       <c r="H251" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="252" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="2" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C252" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D252" s="3">
-        <v>2570000</v>
+        <v>52000000</v>
       </c>
       <c r="E252" s="3">
-        <v>857000</v>
+        <v>13000000</v>
       </c>
       <c r="F252" s="3">
-        <v>10000</v>
+        <v>16000000</v>
       </c>
       <c r="G252" s="3">
-        <v>10000</v>
+        <v>16000000</v>
       </c>
       <c r="H252" s="2" t="s">
-        <v>184</v>
+        <v>46</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="C253" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D253" s="3">
-        <v>13000000</v>
+        <v>51530000</v>
       </c>
       <c r="E253" s="3">
-        <v>6500000</v>
+        <v>17176667</v>
       </c>
       <c r="F253" s="3">
-        <v>7000000</v>
+        <v>30000000</v>
       </c>
       <c r="G253" s="3">
-        <v>7000000</v>
+        <v>30000000</v>
       </c>
       <c r="H253" s="2" t="s">
         <v>17</v>
@@ -8064,103 +8066,103 @@
     </row>
     <row r="254" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="2" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C254" s="2">
         <v>30</v>
       </c>
       <c r="D254" s="3">
-        <v>10500000</v>
+        <v>45000000</v>
       </c>
       <c r="E254" s="3">
-        <v>10500000</v>
+        <v>15000000</v>
       </c>
       <c r="F254" s="3">
-        <v>10500000</v>
+        <v>30000000</v>
       </c>
       <c r="G254" s="3">
-        <v>10500000</v>
+        <v>30000000</v>
       </c>
       <c r="H254" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="255" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="2" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="C255" s="2">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D255" s="3">
-        <v>2500000</v>
+        <v>40000000</v>
       </c>
       <c r="E255" s="3">
-        <v>1250000</v>
+        <v>10000000</v>
       </c>
       <c r="F255" s="3">
-        <v>1000000</v>
+        <v>16000000</v>
       </c>
       <c r="G255" s="3">
-        <v>1000000</v>
+        <v>16000000</v>
       </c>
       <c r="H255" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="256" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="2" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C256" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D256" s="3">
-        <v>5000000</v>
+        <v>2700000</v>
       </c>
       <c r="E256" s="3">
-        <v>1250000</v>
+        <v>900000</v>
       </c>
       <c r="F256" s="3">
-        <v>3000000</v>
+        <v>1080000</v>
       </c>
       <c r="G256" s="3">
-        <v>3000000</v>
+        <v>1080000</v>
       </c>
       <c r="H256" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="257" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="2" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="C257" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D257" s="3">
-        <v>13800000</v>
+        <v>14700000</v>
       </c>
       <c r="E257" s="3">
-        <v>3450000</v>
+        <v>3675000</v>
       </c>
       <c r="F257" s="3">
-        <v>13800000</v>
+        <v>14700000</v>
       </c>
       <c r="G257" s="3">
-        <v>13800000</v>
+        <v>14700000</v>
       </c>
       <c r="H257" s="2" t="s">
         <v>17</v>
@@ -8168,19 +8170,19 @@
     </row>
     <row r="258" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="2" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C258" s="2">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D258" s="3">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="E258" s="3">
-        <v>3000000</v>
+        <v>1250000</v>
       </c>
       <c r="F258" s="3">
         <v>3000000</v>
@@ -8189,128 +8191,128 @@
         <v>3000000</v>
       </c>
       <c r="H258" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="259" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="2" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="C259" s="2">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D259" s="3">
-        <v>4250000</v>
+        <v>2570000</v>
       </c>
       <c r="E259" s="3">
-        <v>4250000</v>
+        <v>857000</v>
       </c>
       <c r="F259" s="3">
-        <v>3000000</v>
+        <v>10000</v>
       </c>
       <c r="G259" s="3">
-        <v>3000000</v>
+        <v>10000</v>
       </c>
       <c r="H259" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="260" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="2" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C260" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D260" s="3">
-        <v>2705000</v>
+        <v>13000000</v>
       </c>
       <c r="E260" s="3">
-        <v>902000</v>
+        <v>6500000</v>
       </c>
       <c r="F260" s="3">
-        <v>45000</v>
+        <v>7000000</v>
       </c>
       <c r="G260" s="3">
-        <v>45000</v>
+        <v>7000000</v>
       </c>
       <c r="H260" s="2" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
     </row>
     <row r="261" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C261" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D261" s="3">
-        <v>21000000</v>
+        <v>10500000</v>
       </c>
       <c r="E261" s="3">
-        <v>7000000</v>
+        <v>10500000</v>
       </c>
       <c r="F261" s="3">
-        <v>16000000</v>
+        <v>10500000</v>
       </c>
       <c r="G261" s="3">
-        <v>16000000</v>
+        <v>10500000</v>
       </c>
       <c r="H261" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="2" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C262" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D262" s="3">
-        <v>5500000</v>
+        <v>2500000</v>
       </c>
       <c r="E262" s="3">
-        <v>2750000</v>
+        <v>1250000</v>
       </c>
       <c r="F262" s="3">
-        <v>2300000</v>
+        <v>1000000</v>
       </c>
       <c r="G262" s="3">
-        <v>2300000</v>
+        <v>1000000</v>
       </c>
       <c r="H262" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="2" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C263" s="2">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D263" s="3">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="E263" s="3">
-        <v>3000000</v>
+        <v>1250000</v>
       </c>
       <c r="F263" s="3">
         <v>3000000</v>
@@ -8319,50 +8321,50 @@
         <v>3000000</v>
       </c>
       <c r="H263" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="2" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="C264" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D264" s="3">
-        <v>2710000</v>
+        <v>13800000</v>
       </c>
       <c r="E264" s="3">
-        <v>903333</v>
+        <v>3450000</v>
       </c>
       <c r="F264" s="3">
-        <v>50000</v>
+        <v>13800000</v>
       </c>
       <c r="G264" s="3">
-        <v>50000</v>
+        <v>13800000</v>
       </c>
       <c r="H264" s="2" t="s">
-        <v>184</v>
+        <v>17</v>
       </c>
     </row>
     <row r="265" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="C265" s="2">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D265" s="3">
-        <v>5200000</v>
+        <v>3000000</v>
       </c>
       <c r="E265" s="3">
-        <v>2600000</v>
+        <v>3000000</v>
       </c>
       <c r="F265" s="3">
         <v>3000000</v>
@@ -8371,134 +8373,134 @@
         <v>3000000</v>
       </c>
       <c r="H265" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="266" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="2" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C266" s="2">
         <v>29</v>
       </c>
       <c r="D266" s="3">
-        <v>43500000</v>
+        <v>4250000</v>
       </c>
       <c r="E266" s="3">
-        <v>14500000</v>
+        <v>4250000</v>
       </c>
       <c r="F266" s="3">
-        <v>30000000</v>
+        <v>3000000</v>
       </c>
       <c r="G266" s="3">
-        <v>30000000</v>
+        <v>3000000</v>
       </c>
       <c r="H266" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="267" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="2" t="s">
-        <v>297</v>
+        <v>334</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C267" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D267" s="3">
-        <v>135000000</v>
+        <v>2705000</v>
       </c>
       <c r="E267" s="3">
-        <v>27000000</v>
+        <v>902000</v>
       </c>
       <c r="F267" s="3">
-        <v>102000000</v>
+        <v>45000</v>
       </c>
       <c r="G267" s="3">
-        <v>78000000</v>
+        <v>45000</v>
       </c>
       <c r="H267" s="2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="268" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>345</v>
+        <v>317</v>
       </c>
       <c r="C268" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D268" s="3">
-        <v>2500000</v>
+        <v>21000000</v>
       </c>
       <c r="E268" s="3">
-        <v>2500000</v>
+        <v>7000000</v>
       </c>
       <c r="F268" s="3">
-        <v>1000000</v>
+        <v>16000000</v>
       </c>
       <c r="G268" s="3">
-        <v>1000000</v>
+        <v>16000000</v>
       </c>
       <c r="H268" s="2" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
     </row>
     <row r="269" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="2" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C269" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D269" s="3">
-        <v>13088000</v>
+        <v>5500000</v>
       </c>
       <c r="E269" s="3">
-        <v>3272000</v>
+        <v>2750000</v>
       </c>
       <c r="F269" s="3">
-        <v>13088000</v>
+        <v>2300000</v>
       </c>
       <c r="G269" s="3">
-        <v>13088000</v>
+        <v>2300000</v>
       </c>
       <c r="H269" s="2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="270" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="2" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C270" s="2">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D270" s="3">
-        <v>2700000</v>
+        <v>3000000</v>
       </c>
       <c r="E270" s="3">
-        <v>900000</v>
+        <v>3000000</v>
       </c>
       <c r="F270" s="3">
-        <v>150000</v>
+        <v>3000000</v>
       </c>
       <c r="G270" s="3">
-        <v>150000</v>
+        <v>3000000</v>
       </c>
       <c r="H270" s="2" t="s">
         <v>52</v>
@@ -8506,54 +8508,80 @@
     </row>
     <row r="271" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="C271" s="2">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D271" s="3">
-        <v>9000000</v>
+        <v>2710000</v>
       </c>
       <c r="E271" s="3">
-        <v>3000000</v>
+        <v>903333</v>
       </c>
       <c r="F271" s="3">
-        <v>3000000</v>
+        <v>50000</v>
       </c>
       <c r="G271" s="3">
-        <v>3000000</v>
+        <v>50000</v>
       </c>
       <c r="H271" s="2" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
     </row>
     <row r="272" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="2" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>307</v>
+        <v>342</v>
       </c>
       <c r="C272" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D272" s="3">
-        <v>2500000</v>
+        <v>5200000</v>
       </c>
       <c r="E272" s="3">
-        <v>833333</v>
+        <v>2600000</v>
       </c>
       <c r="F272" s="3">
-        <v>100000</v>
+        <v>3000000</v>
       </c>
       <c r="G272" s="3">
-        <v>100000</v>
+        <v>3000000</v>
       </c>
       <c r="H272" s="2" t="s">
-        <v>52</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A273" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C273" s="2">
+        <v>29</v>
+      </c>
+      <c r="D273" s="3">
+        <v>43500000</v>
+      </c>
+      <c r="E273" s="3">
+        <v>14500000</v>
+      </c>
+      <c r="F273" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="G273" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="H273" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started to actually build regression models for all salary features.
</commit_message>
<xml_diff>
--- a/Data/SalaryData2024.xlsx
+++ b/Data/SalaryData2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quint\OneDrive\Desktop\Python\PassRusherProfile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301FCFF7-F4E0-4725-B059-9A3709163EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AAF57-E1A0-4F3F-850F-64FA93B7BF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{145E95C2-4CEE-4C00-8587-05CEAAFF428B}"/>
   </bookViews>
@@ -1475,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056453F3-443A-43CE-9113-6295878462E1}">
   <dimension ref="A1:J273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="J252" sqref="J252"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>